<commit_message>
Removed MAPS export, refactored MAP import.
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -8,51 +8,42 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\Programming\Java\viko\2Dgame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C19BEF-841E-4194-AF43-CAF125306926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2389DB-7CCB-4197-9357-158D2DFE5486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21048" yWindow="2280" windowWidth="19200" windowHeight="9108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Maps" sheetId="1" r:id="rId1"/>
+    <sheet name="Map" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Lietuva</t>
   </si>
   <si>
+    <t>Kaunas</t>
+  </si>
+  <si>
+    <t>Siauliai</t>
+  </si>
+  <si>
+    <t>Jonava</t>
+  </si>
+  <si>
+    <t>Klaipeda</t>
+  </si>
+  <si>
+    <t>Cities</t>
+  </si>
+  <si>
     <t>Vilnius</t>
-  </si>
-  <si>
-    <t>Estija</t>
-  </si>
-  <si>
-    <t>Talinas</t>
-  </si>
-  <si>
-    <t>Kaunas</t>
-  </si>
-  <si>
-    <t>Siauliai</t>
-  </si>
-  <si>
-    <t>Jonava</t>
-  </si>
-  <si>
-    <t>Latvija</t>
-  </si>
-  <si>
-    <t>Ventspils</t>
   </si>
 </sst>
 </file>
@@ -404,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,55 +408,35 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>